<commit_message>
last task done. download PDF. More documentation.
</commit_message>
<xml_diff>
--- a/Documentatie/CV_Database.xlsx
+++ b/Documentatie/CV_Database.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Allen\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\CVTemplater\Documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C81BAA3-03C7-49F1-9D7E-94CD990E267A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF31E32D-0352-494E-BE86-58CCC709A815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{96D4EAD7-E983-4C74-B958-76B58F1D381A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="53">
   <si>
     <t>Accounts</t>
   </si>
@@ -44,21 +44,12 @@
     <t>Firstname</t>
   </si>
   <si>
-    <t>User_id</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
     <t>Varchar</t>
   </si>
   <si>
-    <t>Resume_id</t>
-  </si>
-  <si>
     <t>PK INT</t>
   </si>
   <si>
@@ -68,12 +59,6 @@
     <t>Profile</t>
   </si>
   <si>
-    <t>Profile_id</t>
-  </si>
-  <si>
-    <t>Profile_desc</t>
-  </si>
-  <si>
     <t>Birth_date</t>
   </si>
   <si>
@@ -89,84 +74,24 @@
     <t>City</t>
   </si>
   <si>
-    <t>Work_Experience</t>
-  </si>
-  <si>
-    <t>Work_id</t>
-  </si>
-  <si>
     <t>Company</t>
   </si>
   <si>
-    <t>Work_desc</t>
-  </si>
-  <si>
-    <t>Work_title</t>
-  </si>
-  <si>
-    <t>Start_date</t>
-  </si>
-  <si>
-    <t>Leave_date</t>
-  </si>
-  <si>
     <t>Languages</t>
   </si>
   <si>
-    <t>Portfolio</t>
-  </si>
-  <si>
-    <t>Portfolio_id</t>
-  </si>
-  <si>
-    <t>Lang_id</t>
-  </si>
-  <si>
     <t>Contact</t>
   </si>
   <si>
     <t>Phone</t>
   </si>
   <si>
-    <t>Socialmedia2</t>
-  </si>
-  <si>
-    <t>Socialmedia1</t>
-  </si>
-  <si>
-    <t>Socialmedia3</t>
-  </si>
-  <si>
-    <t>Contact_id</t>
-  </si>
-  <si>
     <t>TINYINT</t>
   </si>
   <si>
     <t>Education</t>
   </si>
   <si>
-    <t>Edu_id</t>
-  </si>
-  <si>
-    <t>Edu_title</t>
-  </si>
-  <si>
-    <t>Edu_desc</t>
-  </si>
-  <si>
-    <t>Institute</t>
-  </si>
-  <si>
-    <t>Technical_Skills</t>
-  </si>
-  <si>
-    <t>Tech_id</t>
-  </si>
-  <si>
-    <t>Tech_title</t>
-  </si>
-  <si>
     <t>Username</t>
   </si>
   <si>
@@ -176,15 +101,6 @@
     <t>Lastname</t>
   </si>
   <si>
-    <t>IMG_title</t>
-  </si>
-  <si>
-    <t>IMG_path</t>
-  </si>
-  <si>
-    <t>Profile_intro</t>
-  </si>
-  <si>
     <t>Language</t>
   </si>
   <si>
@@ -194,25 +110,91 @@
     <t>NULL</t>
   </si>
   <si>
-    <t>Boolean</t>
-  </si>
-  <si>
-    <t>Premium</t>
-  </si>
-  <si>
     <t>Resume ID</t>
   </si>
   <si>
-    <t>Resume_title</t>
-  </si>
-  <si>
-    <t>Hobby</t>
-  </si>
-  <si>
-    <t>Hob_id</t>
-  </si>
-  <si>
-    <t>Hobby_entry</t>
+    <t>ResumeID</t>
+  </si>
+  <si>
+    <t>Resumetitle</t>
+  </si>
+  <si>
+    <t>UserID</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>ProfileID</t>
+  </si>
+  <si>
+    <t>Profileintro</t>
+  </si>
+  <si>
+    <t>Profiledesc</t>
+  </si>
+  <si>
+    <t>filePath</t>
+  </si>
+  <si>
+    <t>fileName</t>
+  </si>
+  <si>
+    <t>ContactID</t>
+  </si>
+  <si>
+    <t>firstDate</t>
+  </si>
+  <si>
+    <t>lastDate</t>
+  </si>
+  <si>
+    <t>Technical</t>
+  </si>
+  <si>
+    <t>TechID</t>
+  </si>
+  <si>
+    <t>Techtitle</t>
+  </si>
+  <si>
+    <t>langID</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>Interests</t>
+  </si>
+  <si>
+    <t>interestID</t>
+  </si>
+  <si>
+    <t>interest</t>
+  </si>
+  <si>
+    <t>Experience</t>
+  </si>
+  <si>
+    <t>WorkID</t>
+  </si>
+  <si>
+    <t>Worktitle</t>
+  </si>
+  <si>
+    <t>Workdesc</t>
+  </si>
+  <si>
+    <t>EduID</t>
+  </si>
+  <si>
+    <t>Edutitle</t>
+  </si>
+  <si>
+    <t>Edudesc</t>
+  </si>
+  <si>
+    <t>LangID</t>
   </si>
 </sst>
 </file>
@@ -315,10 +297,10 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right/>
+      <top style="thin">
         <color indexed="64"/>
-      </right>
-      <top/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -328,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -341,8 +323,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -657,10 +649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{362E4F06-5130-4F1B-B6E4-C6E5F104E99F}">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -681,375 +673,391 @@
         <v>0</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="E6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="9" t="s">
-        <v>54</v>
+      <c r="B7" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="D7" s="5"/>
-      <c r="F7" s="4" t="s">
+      <c r="E7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="10" t="s">
         <v>25</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>22</v>
       </c>
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" t="s">
-        <v>50</v>
+        <v>5</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>22</v>
       </c>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G9" t="s">
-        <v>51</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="D10" s="5"/>
-      <c r="E10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G10" t="s">
-        <v>51</v>
+      <c r="F10" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" t="s">
-        <v>51</v>
-      </c>
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
       <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
+      <c r="E11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>22</v>
+      </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" t="s">
-        <v>51</v>
+      <c r="B12" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D12" s="5"/>
-      <c r="F12" s="4" t="s">
-        <v>17</v>
+      <c r="E12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="C18" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="5"/>
+      <c r="A19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>23</v>
+      </c>
       <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="4" t="s">
-        <v>28</v>
+      <c r="A20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
+        <v>23</v>
       </c>
       <c r="D20" s="5"/>
       <c r="F20" s="4" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="H21" s="5"/>
     </row>
@@ -1058,107 +1066,95 @@
         <v>5</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="C22" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" t="s">
-        <v>51</v>
-      </c>
+      <c r="A23" s="12"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
       <c r="D23" s="5"/>
       <c r="E23" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" t="s">
-        <v>51</v>
+      <c r="B24" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>45</v>
+        <v>4</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C26" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="H26" s="5"/>
     </row>
@@ -1167,96 +1163,101 @@
         <v>5</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" t="s">
-        <v>51</v>
+        <v>25</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" t="s">
-        <v>51</v>
+      <c r="B28" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>22</v>
       </c>
       <c r="D28" s="5"/>
-      <c r="F28" s="4" t="s">
-        <v>40</v>
+      <c r="E28" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C29" t="s">
-        <v>51</v>
-      </c>
+      <c r="A29" s="12"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
       <c r="D29" s="5"/>
-      <c r="E29" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G29" t="s">
-        <v>50</v>
-      </c>
+      <c r="E29" s="14"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C30" t="s">
-        <v>51</v>
+      <c r="B30" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="D30" s="5"/>
-      <c r="E30" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F30" s="2" t="s">
+      <c r="F30" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="G30" t="s">
-        <v>51</v>
       </c>
       <c r="H30" s="5"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C31" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
+      <c r="E31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G31" t="s">
+        <v>22</v>
+      </c>
       <c r="H31" s="5"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C32" t="s">
-        <v>51</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>56</v>
+        <v>23</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G32" t="s">
+        <v>23</v>
       </c>
       <c r="H32" s="5"/>
     </row>
@@ -1265,75 +1266,131 @@
         <v>5</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C33" t="s">
-        <v>51</v>
+        <v>25</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G33" t="s">
-        <v>50</v>
+        <v>25</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="H33" s="5"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>22</v>
+      </c>
       <c r="D34" s="5"/>
       <c r="E34" s="3" t="s">
         <v>5</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G34" t="s">
-        <v>51</v>
+        <v>27</v>
+      </c>
+      <c r="G34" s="13" t="s">
+        <v>22</v>
       </c>
       <c r="H34" s="5"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B35" s="4" t="s">
-        <v>24</v>
-      </c>
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
       <c r="D35" s="5"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C36" t="s">
-        <v>50</v>
+      <c r="B36" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="D36" s="5"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C37" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E38" s="5"/>
+      <c r="A38" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" t="s">
+        <v>23</v>
+      </c>
+      <c r="E38" s="14"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="5"/>
+      <c r="A39" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E39" s="14"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="5"/>
+      <c r="A40" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E40" s="14"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E42" s="14"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E43" s="14"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>